<commit_message>
3d 2side dynamic elastic added
</commit_message>
<xml_diff>
--- a/comparison/2story-dynamic-inelastic.xlsx
+++ b/comparison/2story-dynamic-inelastic.xlsx
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -142,6 +142,42 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fa-IR">
+                <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+              </a:rPr>
+              <a:t>جابه جایی پشت</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fa-IR" baseline="0">
+                <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+              </a:rPr>
+              <a:t> بام</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -529,7 +565,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2FC4-4565-8908-12532EEF25E7}"/>
             </c:ext>
@@ -3586,7 +3622,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2FC4-4565-8908-12532EEF25E7}"/>
             </c:ext>
@@ -3600,13 +3636,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="294726800"/>
-        <c:axId val="294727976"/>
+        <c:axId val="382895712"/>
+        <c:axId val="382897672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="294726800"/>
+        <c:axId val="382895712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3624,6 +3661,79 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fa-IR">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>زمان (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>s</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fa-IR">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3661,12 +3771,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="294727976"/>
+        <c:crossAx val="382897672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="294727976"/>
+        <c:axId val="382897672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3686,6 +3796,85 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fa-IR">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>جابه</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fa-IR" baseline="0">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t> جایی (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>cm</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fa-IR" baseline="0">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3723,7 +3912,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="294726800"/>
+        <c:crossAx val="382895712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3805,7 +3994,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3819,6 +4008,42 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fa-IR" b="1">
+                <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+              </a:rPr>
+              <a:t>لنگر خمشی پای</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fa-IR" b="1" baseline="0">
+                <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+              </a:rPr>
+              <a:t> ستون</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1">
+              <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3833,7 +4058,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3842,7 +4067,7 @@
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -4209,7 +4434,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5118-4527-867E-FC6C1280325E}"/>
             </c:ext>
@@ -7266,7 +7491,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5118-4527-867E-FC6C1280325E}"/>
             </c:ext>
@@ -7280,13 +7505,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="378912056"/>
-        <c:axId val="387524056"/>
+        <c:axId val="382889832"/>
+        <c:axId val="382896496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="378912056"/>
+        <c:axId val="382889832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -7304,6 +7530,71 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fa-IR"/>
+                  <a:t>زمان (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>s</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fa-IR"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7341,12 +7632,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387524056"/>
+        <c:crossAx val="382896496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="387524056"/>
+        <c:axId val="382896496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7366,6 +7657,79 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fa-IR">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>لنگر خمشی (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>N.m</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fa-IR">
+                    <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="B Nazanin" panose="00000400000000000000" pitchFamily="2" charset="-78"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7403,7 +7767,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="378912056"/>
+        <c:crossAx val="382889832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7485,7 +7849,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7889,7 +8253,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-70F9-4116-8456-B2137AE370B9}"/>
             </c:ext>
@@ -10946,7 +11310,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-70F9-4116-8456-B2137AE370B9}"/>
             </c:ext>
@@ -10960,11 +11324,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="294727192"/>
-        <c:axId val="294726408"/>
+        <c:axId val="382890224"/>
+        <c:axId val="382898848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="294727192"/>
+        <c:axId val="382890224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11021,12 +11385,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="294726408"/>
+        <c:crossAx val="382898848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="294726408"/>
+        <c:axId val="382898848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11083,7 +11447,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="294727192"/>
+        <c:crossAx val="382890224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12872,15 +13236,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12906,16 +13270,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13231,7 +13595,7 @@
   <dimension ref="A1:D502"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17575,7 +17939,7 @@
   <dimension ref="A1:E502"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23933,7 +24297,7 @@
   <dimension ref="A1:E502"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>